<commit_message>
Updates bancobpi parsing code to accommodate extract header change.
</commit_message>
<xml_diff>
--- a/test/fixtures/cartaobpi_extractados.xlsx
+++ b/test/fixtures/cartaobpi_extractados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ResumoExtracto" sheetId="1" state="visible" r:id="rId2"/>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Desconto</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Transacção</t>
+    <t xml:space="preserve">Data Transação</t>
   </si>
   <si>
     <t xml:space="preserve">Data Movimento</t>
@@ -172,13 +172,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD\-MM\-YYYY;@"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YYYY;@"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY;@"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="0.00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -231,13 +231,6 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
-      <color rgb="FF666666"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -352,7 +345,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -385,19 +378,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -417,7 +406,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,11 +414,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,7 +426,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -445,19 +434,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -542,22 +531,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:43"/>
+  <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="29.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="48.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="17.8469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.66326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="8.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="2" width="9.66326530612245"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="48.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="2" width="9.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5691,11 +5680,11 @@
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
@@ -6725,7 +6714,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
       <c r="D8" s="5"/>
       <c r="H8" s="0"/>
       <c r="I8" s="0"/>
@@ -7749,32 +7738,32 @@
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="n">
+      <c r="B9" s="10" t="n">
         <v>42589</v>
       </c>
       <c r="D9" s="5"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
-      <c r="B10" s="11"/>
+      <c r="B10" s="10"/>
       <c r="D10" s="5"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="n">
+      <c r="B11" s="10" t="n">
         <v>42621</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="0"/>
       <c r="I11" s="0"/>
       <c r="J11" s="0"/>
@@ -8797,27 +8786,27 @@
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="0"/>
       <c r="D13" s="5"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
       <c r="J13" s="0"/>
@@ -9840,14 +9829,14 @@
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="0"/>
       <c r="D14" s="5"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
       <c r="J14" s="0"/>
@@ -10870,14 +10859,14 @@
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="0"/>
       <c r="D15" s="5"/>
       <c r="E15" s="0"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
       <c r="J15" s="0"/>
@@ -11898,12 +11887,12 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
-      <c r="B16" s="8"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="0"/>
       <c r="D16" s="5"/>
       <c r="E16" s="0"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
       <c r="J16" s="0"/>
@@ -12926,14 +12915,14 @@
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="0"/>
       <c r="D17" s="5"/>
       <c r="E17" s="0"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
       <c r="J17" s="0"/>
@@ -13956,14 +13945,14 @@
       <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="0"/>
       <c r="D18" s="5"/>
       <c r="E18" s="0"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="0"/>
       <c r="I18" s="0"/>
       <c r="J18" s="0"/>
@@ -14986,14 +14975,14 @@
       <c r="A19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="0"/>
       <c r="D19" s="5"/>
       <c r="E19" s="0"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="0"/>
       <c r="I19" s="0"/>
       <c r="J19" s="0"/>
@@ -16014,12 +16003,12 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="0"/>
       <c r="D20" s="5"/>
       <c r="E20" s="0"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="0"/>
       <c r="I20" s="0"/>
       <c r="J20" s="0"/>
@@ -17042,11 +17031,11 @@
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="10" t="n">
         <v>42602</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="0"/>
       <c r="I21" s="0"/>
       <c r="J21" s="0"/>
@@ -18069,12 +18058,12 @@
       <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="0"/>
       <c r="I22" s="0"/>
       <c r="J22" s="0"/>
@@ -19094,99 +19083,99 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
       <c r="D23" s="5"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="17"/>
       <c r="D24" s="5"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="14"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="14"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="14"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="5"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="14"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="0"/>
       <c r="D31" s="5"/>
       <c r="E31" s="0"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="0"/>
       <c r="I31" s="0"/>
       <c r="J31" s="0"/>
@@ -20206,13 +20195,13 @@
       <c r="AMJ31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5"/>
       <c r="C32" s="0"/>
       <c r="D32" s="5"/>
       <c r="E32" s="0"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="0"/>
       <c r="I32" s="0"/>
       <c r="J32" s="0"/>
@@ -21232,13 +21221,13 @@
       <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="23"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="7"/>
       <c r="C33" s="0"/>
       <c r="D33" s="5"/>
       <c r="E33" s="0"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
       <c r="H33" s="0"/>
       <c r="I33" s="0"/>
       <c r="J33" s="0"/>
@@ -22264,11 +22253,11 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="24" t="s">
+      <c r="E34" s="11"/>
+      <c r="F34" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="24"/>
       <c r="H34" s="0"/>
       <c r="I34" s="0"/>
       <c r="J34" s="0"/>
@@ -23287,34 +23276,34 @@
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G35" s="25" t="s">
+      <c r="G35" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="27" t="n">
+      <c r="A36" s="26" t="n">
         <v>42588</v>
       </c>
-      <c r="B36" s="27" t="n">
+      <c r="B36" s="26" t="n">
         <v>42590</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -23323,21 +23312,21 @@
       <c r="D36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="12" t="n">
+      <c r="E36" s="11" t="n">
         <v>40</v>
       </c>
-      <c r="F36" s="13" t="n">
+      <c r="F36" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="14" t="n">
+      <c r="G36" s="13" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="27" t="n">
+      <c r="A37" s="26" t="n">
         <v>42586</v>
       </c>
-      <c r="B37" s="27" t="n">
+      <c r="B37" s="26" t="n">
         <v>42590</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -23346,21 +23335,21 @@
       <c r="D37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="12" t="n">
+      <c r="E37" s="11" t="n">
         <v>32.51</v>
       </c>
-      <c r="F37" s="13" t="n">
+      <c r="F37" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G37" s="14" t="n">
+      <c r="G37" s="13" t="n">
         <v>0.33</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="27" t="n">
+      <c r="A38" s="26" t="n">
         <v>42587</v>
       </c>
-      <c r="B38" s="27" t="n">
+      <c r="B38" s="26" t="n">
         <v>42590</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -23369,21 +23358,21 @@
       <c r="D38" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="12" t="n">
+      <c r="E38" s="11" t="n">
         <v>2.99</v>
       </c>
-      <c r="F38" s="13" t="n">
+      <c r="F38" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="14" t="n">
+      <c r="G38" s="13" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="27" t="n">
+      <c r="A39" s="26" t="n">
         <v>42587</v>
       </c>
-      <c r="B39" s="27" t="n">
+      <c r="B39" s="26" t="n">
         <v>42590</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -23392,21 +23381,21 @@
       <c r="D39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="12" t="n">
+      <c r="E39" s="11" t="n">
         <v>146.88</v>
       </c>
-      <c r="F39" s="13" t="n">
+      <c r="F39" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G39" s="14" t="n">
+      <c r="G39" s="13" t="n">
         <v>1.47</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="27" t="n">
+      <c r="A40" s="26" t="n">
         <v>42589</v>
       </c>
-      <c r="B40" s="27" t="n">
+      <c r="B40" s="26" t="n">
         <v>42590</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -23415,21 +23404,21 @@
       <c r="D40" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="12" t="n">
+      <c r="E40" s="11" t="n">
         <v>10.99</v>
       </c>
-      <c r="F40" s="13" t="n">
+      <c r="F40" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G40" s="14" t="n">
+      <c r="G40" s="13" t="n">
         <v>0.11</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="27" t="n">
+      <c r="A41" s="26" t="n">
         <v>42596</v>
       </c>
-      <c r="B41" s="27" t="n">
+      <c r="B41" s="26" t="n">
         <v>42598</v>
       </c>
       <c r="C41" s="5" t="s">
@@ -23438,35 +23427,35 @@
       <c r="D41" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="12" t="n">
+      <c r="E41" s="11" t="n">
         <v>22.21</v>
       </c>
-      <c r="F41" s="13" t="n">
+      <c r="F41" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="G41" s="14" t="n">
+      <c r="G41" s="13" t="n">
         <v>0.22</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="14"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="27"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="14"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -23474,7 +23463,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.708333333333333" right="0.708333333333333" top="0.747916666666667" bottom="0.747916666666667" header="0.315277777777778" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;CDate: &amp;D
 Page &amp;P</oddHeader>

</xml_diff>